<commit_message>
Ad update for LV cells
</commit_message>
<xml_diff>
--- a/Ekran/TouchGFX/assets/texts/texts.xlsx
+++ b/Ekran/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36669" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50670" uniqueCount="951">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2831,6 +2831,108 @@
   <si>
     <t xml:space="preserve">COMMUNICATION
 FAULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pump1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pump2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId821</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId822</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId826</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId833</t>
   </si>
 </sst>
 </file>
@@ -16897,7 +16999,7 @@
         <v>45</v>
       </c>
       <c r="F739" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="740">
@@ -16908,13 +17010,13 @@
         <v>52</v>
       </c>
       <c r="D740" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="E740" t="s">
         <v>45</v>
       </c>
       <c r="F740" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="741">
@@ -16931,7 +17033,7 @@
         <v>45</v>
       </c>
       <c r="F741" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="742">
@@ -16942,13 +17044,13 @@
         <v>52</v>
       </c>
       <c r="D742" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="E742" t="s">
         <v>45</v>
       </c>
       <c r="F742" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="743">
@@ -16965,7 +17067,7 @@
         <v>45</v>
       </c>
       <c r="F743" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="744">
@@ -16982,7 +17084,7 @@
         <v>45</v>
       </c>
       <c r="F744" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="745">
@@ -16993,13 +17095,13 @@
         <v>52</v>
       </c>
       <c r="D745" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="E745" t="s">
         <v>45</v>
       </c>
       <c r="F745" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="746">
@@ -17010,13 +17112,489 @@
         <v>52</v>
       </c>
       <c r="D746" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="E746" t="s">
         <v>45</v>
       </c>
       <c r="F746" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="B747" t="s">
+        <v>917</v>
+      </c>
+      <c r="C747" t="s">
+        <v>52</v>
+      </c>
+      <c r="D747" t="s">
+        <v>44</v>
+      </c>
+      <c r="E747" t="s">
+        <v>45</v>
+      </c>
+      <c r="F747" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="B748" t="s">
+        <v>919</v>
+      </c>
+      <c r="C748" t="s">
+        <v>52</v>
+      </c>
+      <c r="D748" t="s">
+        <v>44</v>
+      </c>
+      <c r="E748" t="s">
+        <v>45</v>
+      </c>
+      <c r="F748" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="B749" t="s">
+        <v>921</v>
+      </c>
+      <c r="C749" t="s">
+        <v>52</v>
+      </c>
+      <c r="D749" t="s">
+        <v>44</v>
+      </c>
+      <c r="E749" t="s">
+        <v>45</v>
+      </c>
+      <c r="F749" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="B750" t="s">
+        <v>923</v>
+      </c>
+      <c r="C750" t="s">
+        <v>52</v>
+      </c>
+      <c r="D750" t="s">
+        <v>44</v>
+      </c>
+      <c r="E750" t="s">
+        <v>45</v>
+      </c>
+      <c r="F750" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="B751" t="s">
+        <v>925</v>
+      </c>
+      <c r="C751" t="s">
+        <v>52</v>
+      </c>
+      <c r="D751" t="s">
+        <v>44</v>
+      </c>
+      <c r="E751" t="s">
+        <v>45</v>
+      </c>
+      <c r="F751" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="B752" t="s">
+        <v>926</v>
+      </c>
+      <c r="C752" t="s">
+        <v>52</v>
+      </c>
+      <c r="D752" t="s">
+        <v>44</v>
+      </c>
+      <c r="E752" t="s">
+        <v>45</v>
+      </c>
+      <c r="F752" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="B753" t="s">
+        <v>927</v>
+      </c>
+      <c r="C753" t="s">
+        <v>52</v>
+      </c>
+      <c r="D753" t="s">
+        <v>44</v>
+      </c>
+      <c r="E753" t="s">
+        <v>45</v>
+      </c>
+      <c r="F753" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="B754" t="s">
+        <v>928</v>
+      </c>
+      <c r="C754" t="s">
+        <v>52</v>
+      </c>
+      <c r="D754" t="s">
+        <v>44</v>
+      </c>
+      <c r="E754" t="s">
+        <v>45</v>
+      </c>
+      <c r="F754" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="B755" t="s">
+        <v>929</v>
+      </c>
+      <c r="C755" t="s">
+        <v>52</v>
+      </c>
+      <c r="D755" t="s">
+        <v>44</v>
+      </c>
+      <c r="E755" t="s">
+        <v>45</v>
+      </c>
+      <c r="F755" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="B756" t="s">
+        <v>930</v>
+      </c>
+      <c r="C756" t="s">
+        <v>52</v>
+      </c>
+      <c r="D756" t="s">
+        <v>44</v>
+      </c>
+      <c r="E756" t="s">
+        <v>45</v>
+      </c>
+      <c r="F756" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="B757" t="s">
+        <v>931</v>
+      </c>
+      <c r="C757" t="s">
+        <v>52</v>
+      </c>
+      <c r="D757" t="s">
+        <v>44</v>
+      </c>
+      <c r="E757" t="s">
+        <v>45</v>
+      </c>
+      <c r="F757" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="B758" t="s">
+        <v>932</v>
+      </c>
+      <c r="C758" t="s">
+        <v>52</v>
+      </c>
+      <c r="D758" t="s">
+        <v>44</v>
+      </c>
+      <c r="E758" t="s">
+        <v>45</v>
+      </c>
+      <c r="F758" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="B759" t="s">
+        <v>933</v>
+      </c>
+      <c r="C759" t="s">
+        <v>52</v>
+      </c>
+      <c r="D759" t="s">
+        <v>44</v>
+      </c>
+      <c r="E759" t="s">
+        <v>45</v>
+      </c>
+      <c r="F759" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="B760" t="s">
+        <v>934</v>
+      </c>
+      <c r="C760" t="s">
+        <v>52</v>
+      </c>
+      <c r="D760" t="s">
+        <v>44</v>
+      </c>
+      <c r="E760" t="s">
+        <v>45</v>
+      </c>
+      <c r="F760" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="B761" t="s">
+        <v>935</v>
+      </c>
+      <c r="C761" t="s">
+        <v>52</v>
+      </c>
+      <c r="D761" t="s">
+        <v>44</v>
+      </c>
+      <c r="E761" t="s">
+        <v>45</v>
+      </c>
+      <c r="F761" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="B762" t="s">
+        <v>936</v>
+      </c>
+      <c r="C762" t="s">
+        <v>52</v>
+      </c>
+      <c r="D762" t="s">
+        <v>44</v>
+      </c>
+      <c r="E762" t="s">
+        <v>45</v>
+      </c>
+      <c r="F762" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="B763" t="s">
+        <v>937</v>
+      </c>
+      <c r="C763" t="s">
+        <v>52</v>
+      </c>
+      <c r="D763" t="s">
+        <v>44</v>
+      </c>
+      <c r="E763" t="s">
+        <v>45</v>
+      </c>
+      <c r="F763" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="B764" t="s">
+        <v>938</v>
+      </c>
+      <c r="C764" t="s">
+        <v>52</v>
+      </c>
+      <c r="D764" t="s">
+        <v>44</v>
+      </c>
+      <c r="E764" t="s">
+        <v>45</v>
+      </c>
+      <c r="F764" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="B765" t="s">
+        <v>939</v>
+      </c>
+      <c r="C765" t="s">
+        <v>52</v>
+      </c>
+      <c r="D765" t="s">
+        <v>44</v>
+      </c>
+      <c r="E765" t="s">
+        <v>45</v>
+      </c>
+      <c r="F765" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="B766" t="s">
+        <v>940</v>
+      </c>
+      <c r="C766" t="s">
+        <v>52</v>
+      </c>
+      <c r="D766" t="s">
+        <v>44</v>
+      </c>
+      <c r="E766" t="s">
+        <v>45</v>
+      </c>
+      <c r="F766" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="B767" t="s">
+        <v>942</v>
+      </c>
+      <c r="C767" t="s">
+        <v>52</v>
+      </c>
+      <c r="D767" t="s">
+        <v>49</v>
+      </c>
+      <c r="E767" t="s">
+        <v>45</v>
+      </c>
+      <c r="F767" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="B768" t="s">
+        <v>943</v>
+      </c>
+      <c r="C768" t="s">
+        <v>52</v>
+      </c>
+      <c r="D768" t="s">
+        <v>44</v>
+      </c>
+      <c r="E768" t="s">
+        <v>45</v>
+      </c>
+      <c r="F768" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="B769" t="s">
+        <v>945</v>
+      </c>
+      <c r="C769" t="s">
+        <v>52</v>
+      </c>
+      <c r="D769" t="s">
+        <v>44</v>
+      </c>
+      <c r="E769" t="s">
+        <v>45</v>
+      </c>
+      <c r="F769" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="B770" t="s">
+        <v>946</v>
+      </c>
+      <c r="C770" t="s">
+        <v>52</v>
+      </c>
+      <c r="D770" t="s">
+        <v>44</v>
+      </c>
+      <c r="E770" t="s">
+        <v>45</v>
+      </c>
+      <c r="F770" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="B771" t="s">
+        <v>947</v>
+      </c>
+      <c r="C771" t="s">
+        <v>52</v>
+      </c>
+      <c r="D771" t="s">
+        <v>49</v>
+      </c>
+      <c r="E771" t="s">
+        <v>45</v>
+      </c>
+      <c r="F771" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="B772" t="s">
+        <v>948</v>
+      </c>
+      <c r="C772" t="s">
+        <v>52</v>
+      </c>
+      <c r="D772" t="s">
+        <v>44</v>
+      </c>
+      <c r="E772" t="s">
+        <v>45</v>
+      </c>
+      <c r="F772" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="B773" t="s">
+        <v>949</v>
+      </c>
+      <c r="C773" t="s">
+        <v>52</v>
+      </c>
+      <c r="D773" t="s">
+        <v>44</v>
+      </c>
+      <c r="E773" t="s">
+        <v>45</v>
+      </c>
+      <c r="F773" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="B774" t="s">
+        <v>950</v>
+      </c>
+      <c r="C774" t="s">
+        <v>52</v>
+      </c>
+      <c r="D774" t="s">
+        <v>44</v>
+      </c>
+      <c r="E774" t="s">
+        <v>45</v>
+      </c>
+      <c r="F774" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sa azuriranim can popisom poruka
</commit_message>
<xml_diff>
--- a/Ekran/TouchGFX/assets/texts/texts.xlsx
+++ b/Ekran/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122774" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215516" uniqueCount="1042">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2966,6 +2966,246 @@
   </si>
   <si>
     <t xml:space="preserve">Cooling system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Fault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECU information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVATING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHARGING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNKNOWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FATAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INVERTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId846</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId847</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XBEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId851</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId856</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precharg info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId869</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">greske</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shutdown info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open/closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fault airMinus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fault airPlus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fault airPlus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreChargeRelay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fault SHD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nije se zatvorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reley closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nije se zatvorio A-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V&lt;95%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nije se zatvorio A+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reley open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not finished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fault SD cmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fault SHD cmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHD cmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage</t>
   </si>
 </sst>
 </file>
@@ -17023,42 +17263,618 @@
         <v>961</v>
       </c>
     </row>
-    <row r="736"/>
-    <row r="737"/>
-    <row r="738"/>
-    <row r="739"/>
-    <row r="740"/>
-    <row r="741"/>
-    <row r="742"/>
-    <row r="743"/>
-    <row r="744"/>
-    <row r="745"/>
-    <row r="746"/>
-    <row r="747"/>
-    <row r="748"/>
-    <row r="749"/>
-    <row r="750"/>
-    <row r="751"/>
-    <row r="752"/>
-    <row r="753"/>
-    <row r="754"/>
-    <row r="755"/>
-    <row r="756"/>
-    <row r="757"/>
-    <row r="758"/>
-    <row r="759"/>
-    <row r="760"/>
-    <row r="761"/>
-    <row r="762"/>
-    <row r="763"/>
-    <row r="764"/>
-    <row r="765"/>
-    <row r="766"/>
-    <row r="767"/>
-    <row r="768"/>
-    <row r="769"/>
-    <row r="770"/>
-    <row r="771"/>
+    <row r="736">
+      <c r="B736" t="s">
+        <v>962</v>
+      </c>
+      <c r="C736" t="s">
+        <v>952</v>
+      </c>
+      <c r="D736" t="s">
+        <v>44</v>
+      </c>
+      <c r="E736" t="s">
+        <v>45</v>
+      </c>
+      <c r="F736" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="B737" t="s">
+        <v>963</v>
+      </c>
+      <c r="C737" t="s">
+        <v>952</v>
+      </c>
+      <c r="D737" t="s">
+        <v>44</v>
+      </c>
+      <c r="E737" t="s">
+        <v>45</v>
+      </c>
+      <c r="F737" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="B738" t="s">
+        <v>966</v>
+      </c>
+      <c r="C738" t="s">
+        <v>52</v>
+      </c>
+      <c r="D738" t="s">
+        <v>44</v>
+      </c>
+      <c r="E738" t="s">
+        <v>45</v>
+      </c>
+      <c r="F738" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="B739" t="s">
+        <v>968</v>
+      </c>
+      <c r="C739" t="s">
+        <v>52</v>
+      </c>
+      <c r="D739" t="s">
+        <v>44</v>
+      </c>
+      <c r="E739" t="s">
+        <v>45</v>
+      </c>
+      <c r="F739" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="B740" t="s">
+        <v>970</v>
+      </c>
+      <c r="C740" t="s">
+        <v>52</v>
+      </c>
+      <c r="D740" t="s">
+        <v>44</v>
+      </c>
+      <c r="E740" t="s">
+        <v>45</v>
+      </c>
+      <c r="F740" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="B741" t="s">
+        <v>972</v>
+      </c>
+      <c r="C741" t="s">
+        <v>52</v>
+      </c>
+      <c r="D741" t="s">
+        <v>44</v>
+      </c>
+      <c r="E741" t="s">
+        <v>45</v>
+      </c>
+      <c r="F741" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="B742" t="s">
+        <v>974</v>
+      </c>
+      <c r="C742" t="s">
+        <v>52</v>
+      </c>
+      <c r="D742" t="s">
+        <v>44</v>
+      </c>
+      <c r="E742" t="s">
+        <v>45</v>
+      </c>
+      <c r="F742" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="B743" t="s">
+        <v>976</v>
+      </c>
+      <c r="C743" t="s">
+        <v>52</v>
+      </c>
+      <c r="D743" t="s">
+        <v>44</v>
+      </c>
+      <c r="E743" t="s">
+        <v>45</v>
+      </c>
+      <c r="F743" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="B744" t="s">
+        <v>977</v>
+      </c>
+      <c r="C744" t="s">
+        <v>52</v>
+      </c>
+      <c r="D744" t="s">
+        <v>44</v>
+      </c>
+      <c r="E744" t="s">
+        <v>45</v>
+      </c>
+      <c r="F744" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="B745" t="s">
+        <v>978</v>
+      </c>
+      <c r="C745" t="s">
+        <v>52</v>
+      </c>
+      <c r="D745" t="s">
+        <v>44</v>
+      </c>
+      <c r="E745" t="s">
+        <v>45</v>
+      </c>
+      <c r="F745" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="B746" t="s">
+        <v>980</v>
+      </c>
+      <c r="C746" t="s">
+        <v>52</v>
+      </c>
+      <c r="D746" t="s">
+        <v>44</v>
+      </c>
+      <c r="E746" t="s">
+        <v>45</v>
+      </c>
+      <c r="F746" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="B747" t="s">
+        <v>982</v>
+      </c>
+      <c r="C747" t="s">
+        <v>52</v>
+      </c>
+      <c r="D747" t="s">
+        <v>44</v>
+      </c>
+      <c r="E747" t="s">
+        <v>45</v>
+      </c>
+      <c r="F747" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="B748" t="s">
+        <v>984</v>
+      </c>
+      <c r="C748" t="s">
+        <v>52</v>
+      </c>
+      <c r="D748" t="s">
+        <v>44</v>
+      </c>
+      <c r="E748" t="s">
+        <v>45</v>
+      </c>
+      <c r="F748" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="B749" t="s">
+        <v>986</v>
+      </c>
+      <c r="C749" t="s">
+        <v>52</v>
+      </c>
+      <c r="D749" t="s">
+        <v>44</v>
+      </c>
+      <c r="E749" t="s">
+        <v>45</v>
+      </c>
+      <c r="F749" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="B750" t="s">
+        <v>988</v>
+      </c>
+      <c r="C750" t="s">
+        <v>52</v>
+      </c>
+      <c r="D750" t="s">
+        <v>44</v>
+      </c>
+      <c r="E750" t="s">
+        <v>45</v>
+      </c>
+      <c r="F750" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="B751" t="s">
+        <v>990</v>
+      </c>
+      <c r="C751" t="s">
+        <v>103</v>
+      </c>
+      <c r="D751" t="s">
+        <v>44</v>
+      </c>
+      <c r="E751" t="s">
+        <v>45</v>
+      </c>
+      <c r="F751" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="B752" t="s">
+        <v>991</v>
+      </c>
+      <c r="C752" t="s">
+        <v>103</v>
+      </c>
+      <c r="D752" t="s">
+        <v>44</v>
+      </c>
+      <c r="E752" t="s">
+        <v>45</v>
+      </c>
+      <c r="F752" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="B753" t="s">
+        <v>996</v>
+      </c>
+      <c r="C753" t="s">
+        <v>952</v>
+      </c>
+      <c r="D753" t="s">
+        <v>49</v>
+      </c>
+      <c r="E753" t="s">
+        <v>45</v>
+      </c>
+      <c r="F753" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="B754" t="s">
+        <v>997</v>
+      </c>
+      <c r="C754" t="s">
+        <v>952</v>
+      </c>
+      <c r="D754" t="s">
+        <v>44</v>
+      </c>
+      <c r="E754" t="s">
+        <v>45</v>
+      </c>
+      <c r="F754" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="B755" t="s">
+        <v>998</v>
+      </c>
+      <c r="C755" t="s">
+        <v>952</v>
+      </c>
+      <c r="D755" t="s">
+        <v>49</v>
+      </c>
+      <c r="E755" t="s">
+        <v>45</v>
+      </c>
+      <c r="F755" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="B756" t="s">
+        <v>999</v>
+      </c>
+      <c r="C756" t="s">
+        <v>952</v>
+      </c>
+      <c r="D756" t="s">
+        <v>44</v>
+      </c>
+      <c r="E756" t="s">
+        <v>45</v>
+      </c>
+      <c r="F756" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="B757" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C757" t="s">
+        <v>952</v>
+      </c>
+      <c r="D757" t="s">
+        <v>44</v>
+      </c>
+      <c r="E757" t="s">
+        <v>45</v>
+      </c>
+      <c r="F757" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="B758" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C758" t="s">
+        <v>952</v>
+      </c>
+      <c r="D758" t="s">
+        <v>44</v>
+      </c>
+      <c r="E758" t="s">
+        <v>45</v>
+      </c>
+      <c r="F758" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="B759" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C759" t="s">
+        <v>952</v>
+      </c>
+      <c r="D759" t="s">
+        <v>44</v>
+      </c>
+      <c r="E759" t="s">
+        <v>45</v>
+      </c>
+      <c r="F759" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="B760" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C760" t="s">
+        <v>38</v>
+      </c>
+      <c r="D760" t="s">
+        <v>44</v>
+      </c>
+      <c r="E760" t="s">
+        <v>45</v>
+      </c>
+      <c r="F760" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="B761" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C761" t="s">
+        <v>38</v>
+      </c>
+      <c r="D761" t="s">
+        <v>44</v>
+      </c>
+      <c r="E761" t="s">
+        <v>45</v>
+      </c>
+      <c r="F761" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="B762" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C762" t="s">
+        <v>952</v>
+      </c>
+      <c r="D762" t="s">
+        <v>44</v>
+      </c>
+      <c r="E762" t="s">
+        <v>45</v>
+      </c>
+      <c r="F762" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="B763" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C763" t="s">
+        <v>952</v>
+      </c>
+      <c r="D763" t="s">
+        <v>44</v>
+      </c>
+      <c r="E763" t="s">
+        <v>45</v>
+      </c>
+      <c r="F763" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="B764" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C764" t="s">
+        <v>38</v>
+      </c>
+      <c r="D764" t="s">
+        <v>44</v>
+      </c>
+      <c r="E764" t="s">
+        <v>45</v>
+      </c>
+      <c r="F764" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="B765" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C765" t="s">
+        <v>38</v>
+      </c>
+      <c r="D765" t="s">
+        <v>44</v>
+      </c>
+      <c r="E765" t="s">
+        <v>45</v>
+      </c>
+      <c r="F765" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="B766" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C766" t="s">
+        <v>38</v>
+      </c>
+      <c r="D766" t="s">
+        <v>44</v>
+      </c>
+      <c r="E766" t="s">
+        <v>45</v>
+      </c>
+      <c r="F766" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="B767" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C767" t="s">
+        <v>38</v>
+      </c>
+      <c r="D767" t="s">
+        <v>44</v>
+      </c>
+      <c r="E767" t="s">
+        <v>45</v>
+      </c>
+      <c r="F767" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="B768" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C768" t="s">
+        <v>952</v>
+      </c>
+      <c r="D768" t="s">
+        <v>44</v>
+      </c>
+      <c r="E768" t="s">
+        <v>45</v>
+      </c>
+      <c r="F768" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="B769" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C769" t="s">
+        <v>38</v>
+      </c>
+      <c r="D769" t="s">
+        <v>44</v>
+      </c>
+      <c r="E769" t="s">
+        <v>45</v>
+      </c>
+      <c r="F769" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="B770" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C770" t="s">
+        <v>952</v>
+      </c>
+      <c r="D770" t="s">
+        <v>44</v>
+      </c>
+      <c r="E770" t="s">
+        <v>45</v>
+      </c>
+      <c r="F770" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="B771" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C771" t="s">
+        <v>952</v>
+      </c>
+      <c r="D771" t="s">
+        <v>44</v>
+      </c>
+      <c r="E771" t="s">
+        <v>45</v>
+      </c>
+      <c r="F771" t="s">
+        <v>1035</v>
+      </c>
+    </row>
     <row r="772"/>
     <row r="773"/>
     <row r="774"/>

</xml_diff>

<commit_message>
update can popis poruka
</commit_message>
<xml_diff>
--- a/Ekran/TouchGFX/assets/texts/texts.xlsx
+++ b/Ekran/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215516" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262598" uniqueCount="1065">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3206,6 +3206,75 @@
   </si>
   <si>
     <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatal error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vol:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curr:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId889</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId891</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuator fault code:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId894</t>
   </si>
 </sst>
 </file>
@@ -16682,7 +16751,7 @@
         <v>45</v>
       </c>
       <c r="F701" t="s">
-        <v>79</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="702">
@@ -16733,7 +16802,7 @@
         <v>45</v>
       </c>
       <c r="F704" t="s">
-        <v>951</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="705">
@@ -17532,7 +17601,7 @@
         <v>45</v>
       </c>
       <c r="F751" t="s">
-        <v>256</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="752">
@@ -17549,7 +17618,7 @@
         <v>45</v>
       </c>
       <c r="F752" t="s">
-        <v>261</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="753">
@@ -17770,7 +17839,7 @@
         <v>45</v>
       </c>
       <c r="F765" t="s">
-        <v>1039</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="766">
@@ -17875,9 +17944,193 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="772"/>
-    <row r="773"/>
-    <row r="774"/>
+    <row r="772">
+      <c r="B772" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C772" t="s">
+        <v>103</v>
+      </c>
+      <c r="D772" t="s">
+        <v>44</v>
+      </c>
+      <c r="E772" t="s">
+        <v>45</v>
+      </c>
+      <c r="F772" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="B773" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C773" t="s">
+        <v>103</v>
+      </c>
+      <c r="D773" t="s">
+        <v>44</v>
+      </c>
+      <c r="E773" t="s">
+        <v>45</v>
+      </c>
+      <c r="F773" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="B774" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C774" t="s">
+        <v>103</v>
+      </c>
+      <c r="D774" t="s">
+        <v>44</v>
+      </c>
+      <c r="E774" t="s">
+        <v>45</v>
+      </c>
+      <c r="F774" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="B775" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C775" t="s">
+        <v>952</v>
+      </c>
+      <c r="D775" t="s">
+        <v>44</v>
+      </c>
+      <c r="E775" t="s">
+        <v>45</v>
+      </c>
+      <c r="F775" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="B776" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C776" t="s">
+        <v>103</v>
+      </c>
+      <c r="D776" t="s">
+        <v>44</v>
+      </c>
+      <c r="E776" t="s">
+        <v>45</v>
+      </c>
+      <c r="F776" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="B777" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C777" t="s">
+        <v>52</v>
+      </c>
+      <c r="D777" t="s">
+        <v>44</v>
+      </c>
+      <c r="E777" t="s">
+        <v>45</v>
+      </c>
+      <c r="F777" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="B778" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C778" t="s">
+        <v>955</v>
+      </c>
+      <c r="D778" t="s">
+        <v>44</v>
+      </c>
+      <c r="E778" t="s">
+        <v>45</v>
+      </c>
+      <c r="F778" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="B779" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C779" t="s">
+        <v>955</v>
+      </c>
+      <c r="D779" t="s">
+        <v>44</v>
+      </c>
+      <c r="E779" t="s">
+        <v>45</v>
+      </c>
+      <c r="F779" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="B780" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C780" t="s">
+        <v>38</v>
+      </c>
+      <c r="D780" t="s">
+        <v>44</v>
+      </c>
+      <c r="E780" t="s">
+        <v>45</v>
+      </c>
+      <c r="F780" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="B781" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C781" t="s">
+        <v>41</v>
+      </c>
+      <c r="D781" t="s">
+        <v>49</v>
+      </c>
+      <c r="E781" t="s">
+        <v>45</v>
+      </c>
+      <c r="F781" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="B782" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C782" t="s">
+        <v>41</v>
+      </c>
+      <c r="D782" t="s">
+        <v>44</v>
+      </c>
+      <c r="E782" t="s">
+        <v>45</v>
+      </c>
+      <c r="F782" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>